<commit_message>
- generated larger subsets of mnist data - saved the dictionary for dp for these subsets - generated the classification results for these subsets using active learning based nn classification
</commit_message>
<xml_diff>
--- a/output/to_publish/results12.xlsx
+++ b/output/to_publish/results12.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="55">
   <si>
     <t>Dataset</t>
   </si>
@@ -151,6 +151,42 @@
   </si>
   <si>
     <t>mnist2-deskewed - #points = 2000, #features=784</t>
+  </si>
+  <si>
+    <t>mnist3-deskewed</t>
+  </si>
+  <si>
+    <t>mnist4-deskewed</t>
+  </si>
+  <si>
+    <t>mnist3-deskewed - #points = 5000, #features=784</t>
+  </si>
+  <si>
+    <t>dp-max (3383)</t>
+  </si>
+  <si>
+    <t>dp-mean (2301)</t>
+  </si>
+  <si>
+    <t>mnist4-deskewed - #points = 10000, #features=784</t>
+  </si>
+  <si>
+    <t>dp-max (6732)</t>
+  </si>
+  <si>
+    <t>dp-mean (4609)</t>
+  </si>
+  <si>
+    <t>randomized (3383)</t>
+  </si>
+  <si>
+    <t>randomized (2301)</t>
+  </si>
+  <si>
+    <t>randomized (6732)</t>
+  </si>
+  <si>
+    <t>randomized (4609)</t>
   </si>
 </sst>
 </file>
@@ -1058,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H164"/>
+  <dimension ref="A1:Q165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,9 +1108,15 @@
     <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>42</v>
       </c>
@@ -1084,8 +1126,17 @@
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1105,8 +1156,27 @@
       <c r="G2" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -1126,8 +1196,27 @@
       <c r="G3" s="8">
         <v>11.11111</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="5">
+        <v>45</v>
+      </c>
+      <c r="K3" s="8">
+        <v>4.5763800000000003</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="5">
+        <v>45</v>
+      </c>
+      <c r="O3" s="8">
+        <v>6.1842899999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1147,8 +1236,27 @@
       <c r="G4" s="8">
         <v>10.172140000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="5">
+        <v>40</v>
+      </c>
+      <c r="K4" s="8">
+        <v>2.4737200000000001</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="5">
+        <v>40</v>
+      </c>
+      <c r="O4" s="8">
+        <v>5.8750799999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1168,8 +1276,27 @@
       <c r="G5" s="8">
         <v>9.54617</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5">
+        <v>35</v>
+      </c>
+      <c r="K5" s="8">
+        <v>2.0408200000000001</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="5">
+        <v>35</v>
+      </c>
+      <c r="O5" s="8">
+        <v>5.6895499999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1189,8 +1316,27 @@
       <c r="G6" s="8">
         <v>8.4506999999999994</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="5">
+        <v>30</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1.5460700000000001</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="5">
+        <v>30</v>
+      </c>
+      <c r="O6" s="8">
+        <v>5.0092800000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1210,8 +1356,27 @@
       <c r="G7" s="8">
         <v>8.4506999999999994</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="5">
+        <v>25</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1.2987</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="5">
+        <v>25</v>
+      </c>
+      <c r="O7" s="8">
+        <v>4.9474299999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -1231,8 +1396,27 @@
       <c r="G8" s="8">
         <v>8.1377199999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="5">
+        <v>20</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.98948999999999998</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="5">
+        <v>20</v>
+      </c>
+      <c r="O8" s="8">
+        <v>4.5145299999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1252,8 +1436,27 @@
       <c r="G9" s="8">
         <v>6.72926</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="5">
+        <v>15</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0.80396000000000001</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="5">
+        <v>15</v>
+      </c>
+      <c r="O9" s="8">
+        <v>4.1434800000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1273,8 +1476,27 @@
       <c r="G10" s="8">
         <v>6.2597800000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="5">
+        <v>10</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0.61843000000000004</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="5">
+        <v>10</v>
+      </c>
+      <c r="O10" s="8">
+        <v>3.7105800000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -1294,8 +1516,27 @@
       <c r="G11" s="8">
         <v>5.0078199999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="5">
+        <v>5</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0.92764000000000002</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="5">
+        <v>5</v>
+      </c>
+      <c r="O11" s="8">
+        <v>3.8961000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
@@ -1315,8 +1556,27 @@
       <c r="G12" s="11">
         <v>4.8513299999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0.92764000000000002</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="5">
+        <v>1</v>
+      </c>
+      <c r="O12" s="11">
+        <v>3.83426</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>25</v>
       </c>
@@ -1336,8 +1596,27 @@
       <c r="G13" s="8">
         <v>14.455780000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="5">
+        <v>45</v>
+      </c>
+      <c r="K13" s="8">
+        <v>22.37866</v>
+      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="5">
+        <v>45</v>
+      </c>
+      <c r="O13" s="8">
+        <v>9.2997399999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -1357,8 +1636,27 @@
       <c r="G14" s="8">
         <v>13.775510000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="5">
+        <v>40</v>
+      </c>
+      <c r="K14" s="8">
+        <v>20.56317</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="5">
+        <v>40</v>
+      </c>
+      <c r="O14" s="8">
+        <v>9.1885899999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -1378,8 +1676,27 @@
       <c r="G15" s="8">
         <v>13.09524</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="5">
+        <v>35</v>
+      </c>
+      <c r="K15" s="8">
+        <v>17.710260000000002</v>
+      </c>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" s="5">
+        <v>35</v>
+      </c>
+      <c r="O15" s="8">
+        <v>8.2993699999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -1399,8 +1716,27 @@
       <c r="G16" s="8">
         <v>12.41497</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="5">
+        <v>30</v>
+      </c>
+      <c r="K16" s="8">
+        <v>15.005559999999999</v>
+      </c>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N16" s="5">
+        <v>30</v>
+      </c>
+      <c r="O16" s="8">
+        <v>7.5213000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
@@ -1420,8 +1756,27 @@
       <c r="G17" s="8">
         <v>12.15986</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="5">
+        <v>25</v>
+      </c>
+      <c r="K17" s="8">
+        <v>12.337899999999999</v>
+      </c>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N17" s="5">
+        <v>25</v>
+      </c>
+      <c r="O17" s="8">
+        <v>7.0396400000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -1441,8 +1796,27 @@
       <c r="G18" s="8">
         <v>11.39456</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="5">
+        <v>20</v>
+      </c>
+      <c r="K18" s="8">
+        <v>9.4108900000000002</v>
+      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" s="5">
+        <v>20</v>
+      </c>
+      <c r="O18" s="8">
+        <v>6.7432400000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
@@ -1462,8 +1836,27 @@
       <c r="G19" s="8">
         <v>10.45918</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="5">
+        <v>15</v>
+      </c>
+      <c r="K19" s="8">
+        <v>6.2615800000000004</v>
+      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N19" s="5">
+        <v>15</v>
+      </c>
+      <c r="O19" s="8">
+        <v>5.8540200000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -1483,8 +1876,27 @@
       <c r="G20" s="8">
         <v>9.0986399999999996</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="5">
+        <v>10</v>
+      </c>
+      <c r="K20" s="8">
+        <v>2.4083000000000001</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N20" s="5">
+        <v>10</v>
+      </c>
+      <c r="O20" s="8">
+        <v>5.2241600000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1504,8 +1916,27 @@
       <c r="G21" s="8">
         <v>7.1428599999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="5">
+        <v>5</v>
+      </c>
+      <c r="K21" s="11">
+        <v>2.2971499999999998</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N21" s="5">
+        <v>5</v>
+      </c>
+      <c r="O21" s="8">
+        <v>4.7054499999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -1525,8 +1956,27 @@
       <c r="G22" s="11">
         <v>6.2925199999999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="5">
+        <v>1</v>
+      </c>
+      <c r="K22" s="8">
+        <v>2.9270100000000001</v>
+      </c>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N22" s="5">
+        <v>1</v>
+      </c>
+      <c r="O22" s="11">
+        <v>4.3719900000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>26</v>
       </c>
@@ -1547,7 +1997,7 @@
         <v>22.286449999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
@@ -1568,7 +2018,7 @@
         <v>20.680800000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
@@ -1588,8 +2038,17 @@
       <c r="G25" s="8">
         <v>18.689789999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I25" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
@@ -1609,8 +2068,27 @@
       <c r="G26" s="8">
         <v>16.891459999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1630,8 +2108,27 @@
       <c r="G27" s="8">
         <v>15.221579999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J27" s="5">
+        <v>45</v>
+      </c>
+      <c r="K27" s="8">
+        <v>1.8971800000000001</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N27" s="5">
+        <v>45</v>
+      </c>
+      <c r="O27" s="8">
+        <v>6.7931499999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>9</v>
       </c>
@@ -1651,8 +2148,27 @@
       <c r="G28" s="8">
         <v>13.423249999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J28" s="5">
+        <v>40</v>
+      </c>
+      <c r="K28" s="8">
+        <v>1.7441899999999999</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N28" s="5">
+        <v>40</v>
+      </c>
+      <c r="O28" s="8">
+        <v>6.6095499999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>9</v>
       </c>
@@ -1672,8 +2188,27 @@
       <c r="G29" s="8">
         <v>11.046889999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" s="5">
+        <v>35</v>
+      </c>
+      <c r="K29" s="8">
+        <v>1.6217900000000001</v>
+      </c>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N29" s="5">
+        <v>35</v>
+      </c>
+      <c r="O29" s="8">
+        <v>6.1811499999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>9</v>
       </c>
@@ -1693,8 +2228,27 @@
       <c r="G30" s="8">
         <v>9.5054599999999994</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" s="5">
+        <v>30</v>
+      </c>
+      <c r="K30" s="8">
+        <v>1.34639</v>
+      </c>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N30" s="5">
+        <v>30</v>
+      </c>
+      <c r="O30" s="8">
+        <v>5.93635</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>9</v>
       </c>
@@ -1714,8 +2268,27 @@
       <c r="G31" s="8">
         <v>8.4136199999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J31" s="5">
+        <v>25</v>
+      </c>
+      <c r="K31" s="8">
+        <v>1.13219</v>
+      </c>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N31" s="5">
+        <v>25</v>
+      </c>
+      <c r="O31" s="8">
+        <v>5.47736</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>9</v>
       </c>
@@ -1735,8 +2308,27 @@
       <c r="G32" s="11">
         <v>8.73475</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" s="5">
+        <v>20</v>
+      </c>
+      <c r="K32" s="8">
+        <v>1.0403899999999999</v>
+      </c>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N32" s="5">
+        <v>20</v>
+      </c>
+      <c r="O32" s="8">
+        <v>4.8959599999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>27</v>
       </c>
@@ -1756,8 +2348,27 @@
       <c r="G33" s="8">
         <v>22.1374</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J33" s="5">
+        <v>15</v>
+      </c>
+      <c r="K33" s="8">
+        <v>0.88739000000000001</v>
+      </c>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N33" s="5">
+        <v>15</v>
+      </c>
+      <c r="O33" s="8">
+        <v>4.4063600000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>10</v>
       </c>
@@ -1777,8 +2388,27 @@
       <c r="G34" s="8">
         <v>20.992370000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="5">
+        <v>10</v>
+      </c>
+      <c r="K34" s="8">
+        <v>0.70379000000000003</v>
+      </c>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N34" s="5">
+        <v>10</v>
+      </c>
+      <c r="O34" s="8">
+        <v>3.9167700000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>10</v>
       </c>
@@ -1798,8 +2428,27 @@
       <c r="G35" s="8">
         <v>19.338419999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I35" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="5">
+        <v>5</v>
+      </c>
+      <c r="K35" s="8">
+        <v>0.76498999999999995</v>
+      </c>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N35" s="5">
+        <v>5</v>
+      </c>
+      <c r="O35" s="8">
+        <v>3.7025700000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>10</v>
       </c>
@@ -1819,8 +2468,27 @@
       <c r="G36" s="8">
         <v>17.048349999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="5">
+        <v>1</v>
+      </c>
+      <c r="K36" s="11">
+        <v>0.5202</v>
+      </c>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N36" s="5">
+        <v>1</v>
+      </c>
+      <c r="O36" s="11">
+        <v>3.3965700000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>10</v>
       </c>
@@ -1840,8 +2508,27 @@
       <c r="G37" s="8">
         <v>15.458019999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I37" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J37" s="5">
+        <v>45</v>
+      </c>
+      <c r="K37" s="8">
+        <v>11.05546</v>
+      </c>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N37" s="5">
+        <v>45</v>
+      </c>
+      <c r="O37" s="8">
+        <v>6.3624599999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>10</v>
       </c>
@@ -1861,8 +2548,27 @@
       <c r="G38" s="8">
         <v>13.549620000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" s="5">
+        <v>40</v>
+      </c>
+      <c r="K38" s="8">
+        <v>7.9762599999999999</v>
+      </c>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N38" s="5">
+        <v>40</v>
+      </c>
+      <c r="O38" s="8">
+        <v>6.1955099999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>10</v>
       </c>
@@ -1882,8 +2588,27 @@
       <c r="G39" s="8">
         <v>11.259539999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" s="5">
+        <v>35</v>
+      </c>
+      <c r="K39" s="8">
+        <v>5.6575800000000003</v>
+      </c>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N39" s="5">
+        <v>35</v>
+      </c>
+      <c r="O39" s="8">
+        <v>5.8801699999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>10</v>
       </c>
@@ -1903,8 +2628,27 @@
       <c r="G40" s="8">
         <v>9.47837</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J40" s="5">
+        <v>30</v>
+      </c>
+      <c r="K40" s="8">
+        <v>4.13652</v>
+      </c>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N40" s="5">
+        <v>30</v>
+      </c>
+      <c r="O40" s="8">
+        <v>5.58338</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>10</v>
       </c>
@@ -1924,8 +2668,27 @@
       <c r="G41" s="8">
         <v>8.3969500000000004</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J41" s="5">
+        <v>25</v>
+      </c>
+      <c r="K41" s="8">
+        <v>3.4316499999999999</v>
+      </c>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N41" s="5">
+        <v>25</v>
+      </c>
+      <c r="O41" s="8">
+        <v>5.4349800000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>10</v>
       </c>
@@ -1945,8 +2708,27 @@
       <c r="G42" s="11">
         <v>9.0966900000000006</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I42" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J42" s="5">
+        <v>20</v>
+      </c>
+      <c r="K42" s="8">
+        <v>3.0235599999999998</v>
+      </c>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N42" s="5">
+        <v>20</v>
+      </c>
+      <c r="O42" s="8">
+        <v>4.9341499999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
@@ -1966,8 +2748,27 @@
       <c r="G43" s="8">
         <v>12.950340000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J43" s="5">
+        <v>15</v>
+      </c>
+      <c r="K43" s="8">
+        <v>2.3001299999999998</v>
+      </c>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N43" s="5">
+        <v>15</v>
+      </c>
+      <c r="O43" s="8">
+        <v>4.7115600000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>12</v>
       </c>
@@ -1987,8 +2788,27 @@
       <c r="G44" s="8">
         <v>12.17137</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J44" s="5">
+        <v>10</v>
+      </c>
+      <c r="K44" s="8">
+        <v>1.83639</v>
+      </c>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N44" s="5">
+        <v>10</v>
+      </c>
+      <c r="O44" s="8">
+        <v>4.2663700000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>12</v>
       </c>
@@ -2008,8 +2828,27 @@
       <c r="G45" s="8">
         <v>11.295030000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J45" s="5">
+        <v>5</v>
+      </c>
+      <c r="K45" s="11">
+        <v>1.7436499999999999</v>
+      </c>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N45" s="5">
+        <v>5</v>
+      </c>
+      <c r="O45" s="8">
+        <v>4.0623300000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>12</v>
       </c>
@@ -2029,8 +2868,27 @@
       <c r="G46" s="8">
         <v>10.32132</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J46" s="5">
+        <v>1</v>
+      </c>
+      <c r="K46" s="8">
+        <v>1.9291400000000001</v>
+      </c>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N46" s="5">
+        <v>1</v>
+      </c>
+      <c r="O46" s="11">
+        <v>3.9139300000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>12</v>
       </c>
@@ -2051,7 +2909,7 @@
         <v>10.029210000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>12</v>
       </c>
@@ -2744,7 +3602,7 @@
         <v>19.789940000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>15</v>
       </c>
@@ -2765,7 +3623,7 @@
         <v>15.03593</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>15</v>
       </c>
@@ -2786,7 +3644,7 @@
         <v>12.935320000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>18</v>
       </c>
@@ -2812,7 +3670,7 @@
         <v>32.237870000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>18</v>
       </c>
@@ -2837,8 +3695,32 @@
       <c r="H86">
         <v>28.325510000000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J86" t="s">
+        <v>43</v>
+      </c>
+      <c r="K86" t="s">
+        <v>8</v>
+      </c>
+      <c r="L86">
+        <v>5000</v>
+      </c>
+      <c r="M86">
+        <v>784</v>
+      </c>
+      <c r="N86">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O86">
+        <v>3383</v>
+      </c>
+      <c r="P86">
+        <v>45</v>
+      </c>
+      <c r="Q86">
+        <v>4.5763800000000003</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>18</v>
       </c>
@@ -2863,8 +3745,32 @@
       <c r="H87">
         <v>24.25665</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J87" t="s">
+        <v>43</v>
+      </c>
+      <c r="K87" t="s">
+        <v>8</v>
+      </c>
+      <c r="L87">
+        <v>5000</v>
+      </c>
+      <c r="M87">
+        <v>784</v>
+      </c>
+      <c r="N87">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O87">
+        <v>3383</v>
+      </c>
+      <c r="P87">
+        <v>40</v>
+      </c>
+      <c r="Q87">
+        <v>2.4737200000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>18</v>
       </c>
@@ -2889,8 +3795,32 @@
       <c r="H88">
         <v>20.500779999999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J88" t="s">
+        <v>43</v>
+      </c>
+      <c r="K88" t="s">
+        <v>8</v>
+      </c>
+      <c r="L88">
+        <v>5000</v>
+      </c>
+      <c r="M88">
+        <v>784</v>
+      </c>
+      <c r="N88">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O88">
+        <v>3383</v>
+      </c>
+      <c r="P88">
+        <v>35</v>
+      </c>
+      <c r="Q88">
+        <v>2.0408200000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>18</v>
       </c>
@@ -2915,8 +3845,32 @@
       <c r="H89">
         <v>16.27543</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J89" t="s">
+        <v>43</v>
+      </c>
+      <c r="K89" t="s">
+        <v>8</v>
+      </c>
+      <c r="L89">
+        <v>5000</v>
+      </c>
+      <c r="M89">
+        <v>784</v>
+      </c>
+      <c r="N89">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O89">
+        <v>3383</v>
+      </c>
+      <c r="P89">
+        <v>30</v>
+      </c>
+      <c r="Q89">
+        <v>1.5460700000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>18</v>
       </c>
@@ -2941,8 +3895,32 @@
       <c r="H90">
         <v>13.30203</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J90" t="s">
+        <v>43</v>
+      </c>
+      <c r="K90" t="s">
+        <v>8</v>
+      </c>
+      <c r="L90">
+        <v>5000</v>
+      </c>
+      <c r="M90">
+        <v>784</v>
+      </c>
+      <c r="N90">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O90">
+        <v>3383</v>
+      </c>
+      <c r="P90">
+        <v>25</v>
+      </c>
+      <c r="Q90">
+        <v>1.2987</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>18</v>
       </c>
@@ -2967,8 +3945,32 @@
       <c r="H91">
         <v>5.3208099999999998</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J91" t="s">
+        <v>43</v>
+      </c>
+      <c r="K91" t="s">
+        <v>8</v>
+      </c>
+      <c r="L91">
+        <v>5000</v>
+      </c>
+      <c r="M91">
+        <v>784</v>
+      </c>
+      <c r="N91">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O91">
+        <v>3383</v>
+      </c>
+      <c r="P91">
+        <v>20</v>
+      </c>
+      <c r="Q91">
+        <v>0.98948999999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -2993,8 +3995,32 @@
       <c r="H92">
         <v>1.25196</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J92" t="s">
+        <v>43</v>
+      </c>
+      <c r="K92" t="s">
+        <v>8</v>
+      </c>
+      <c r="L92">
+        <v>5000</v>
+      </c>
+      <c r="M92">
+        <v>784</v>
+      </c>
+      <c r="N92">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O92">
+        <v>3383</v>
+      </c>
+      <c r="P92">
+        <v>15</v>
+      </c>
+      <c r="Q92">
+        <v>0.80396000000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>18</v>
       </c>
@@ -3019,8 +4045,32 @@
       <c r="H93">
         <v>0.93896999999999997</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J93" t="s">
+        <v>43</v>
+      </c>
+      <c r="K93" t="s">
+        <v>8</v>
+      </c>
+      <c r="L93">
+        <v>5000</v>
+      </c>
+      <c r="M93">
+        <v>784</v>
+      </c>
+      <c r="N93">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O93">
+        <v>3383</v>
+      </c>
+      <c r="P93">
+        <v>10</v>
+      </c>
+      <c r="Q93">
+        <v>0.61843000000000004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>18</v>
       </c>
@@ -3045,8 +4095,32 @@
       <c r="H94">
         <v>1.25196</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J94" t="s">
+        <v>43</v>
+      </c>
+      <c r="K94" t="s">
+        <v>8</v>
+      </c>
+      <c r="L94">
+        <v>5000</v>
+      </c>
+      <c r="M94">
+        <v>784</v>
+      </c>
+      <c r="N94">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O94">
+        <v>3383</v>
+      </c>
+      <c r="P94">
+        <v>5</v>
+      </c>
+      <c r="Q94">
+        <v>0.92764000000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>18</v>
       </c>
@@ -3071,8 +4145,32 @@
       <c r="H95">
         <v>21.59864</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J95" t="s">
+        <v>43</v>
+      </c>
+      <c r="K95" t="s">
+        <v>8</v>
+      </c>
+      <c r="L95">
+        <v>5000</v>
+      </c>
+      <c r="M95">
+        <v>784</v>
+      </c>
+      <c r="N95">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O95">
+        <v>3383</v>
+      </c>
+      <c r="P95">
+        <v>1</v>
+      </c>
+      <c r="Q95">
+        <v>0.92764000000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>18</v>
       </c>
@@ -3097,8 +4195,32 @@
       <c r="H96">
         <v>17.94218</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J96" t="s">
+        <v>43</v>
+      </c>
+      <c r="K96" t="s">
+        <v>12</v>
+      </c>
+      <c r="L96">
+        <v>5000</v>
+      </c>
+      <c r="M96">
+        <v>784</v>
+      </c>
+      <c r="N96">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O96">
+        <v>2301</v>
+      </c>
+      <c r="P96">
+        <v>45</v>
+      </c>
+      <c r="Q96">
+        <v>22.37866</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>18</v>
       </c>
@@ -3123,8 +4245,32 @@
       <c r="H97">
         <v>15.136049999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J97" t="s">
+        <v>43</v>
+      </c>
+      <c r="K97" t="s">
+        <v>12</v>
+      </c>
+      <c r="L97">
+        <v>5000</v>
+      </c>
+      <c r="M97">
+        <v>784</v>
+      </c>
+      <c r="N97">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O97">
+        <v>2301</v>
+      </c>
+      <c r="P97">
+        <v>40</v>
+      </c>
+      <c r="Q97">
+        <v>20.56317</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>18</v>
       </c>
@@ -3149,8 +4295,32 @@
       <c r="H98">
         <v>11.309519999999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J98" t="s">
+        <v>43</v>
+      </c>
+      <c r="K98" t="s">
+        <v>12</v>
+      </c>
+      <c r="L98">
+        <v>5000</v>
+      </c>
+      <c r="M98">
+        <v>784</v>
+      </c>
+      <c r="N98">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O98">
+        <v>2301</v>
+      </c>
+      <c r="P98">
+        <v>35</v>
+      </c>
+      <c r="Q98">
+        <v>17.710260000000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>18</v>
       </c>
@@ -3175,8 +4345,32 @@
       <c r="H99">
         <v>8.5033999999999992</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J99" t="s">
+        <v>43</v>
+      </c>
+      <c r="K99" t="s">
+        <v>12</v>
+      </c>
+      <c r="L99">
+        <v>5000</v>
+      </c>
+      <c r="M99">
+        <v>784</v>
+      </c>
+      <c r="N99">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O99">
+        <v>2301</v>
+      </c>
+      <c r="P99">
+        <v>30</v>
+      </c>
+      <c r="Q99">
+        <v>15.005559999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>18</v>
       </c>
@@ -3201,8 +4395,32 @@
       <c r="H100">
         <v>6.1224499999999997</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J100" t="s">
+        <v>43</v>
+      </c>
+      <c r="K100" t="s">
+        <v>12</v>
+      </c>
+      <c r="L100">
+        <v>5000</v>
+      </c>
+      <c r="M100">
+        <v>784</v>
+      </c>
+      <c r="N100">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O100">
+        <v>2301</v>
+      </c>
+      <c r="P100">
+        <v>25</v>
+      </c>
+      <c r="Q100">
+        <v>12.337899999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>18</v>
       </c>
@@ -3227,8 +4445,32 @@
       <c r="H101">
         <v>3.4863900000000001</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J101" t="s">
+        <v>43</v>
+      </c>
+      <c r="K101" t="s">
+        <v>12</v>
+      </c>
+      <c r="L101">
+        <v>5000</v>
+      </c>
+      <c r="M101">
+        <v>784</v>
+      </c>
+      <c r="N101">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O101">
+        <v>2301</v>
+      </c>
+      <c r="P101">
+        <v>20</v>
+      </c>
+      <c r="Q101">
+        <v>9.4108900000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>18</v>
       </c>
@@ -3253,8 +4495,32 @@
       <c r="H102">
         <v>3.23129</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J102" t="s">
+        <v>43</v>
+      </c>
+      <c r="K102" t="s">
+        <v>12</v>
+      </c>
+      <c r="L102">
+        <v>5000</v>
+      </c>
+      <c r="M102">
+        <v>784</v>
+      </c>
+      <c r="N102">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O102">
+        <v>2301</v>
+      </c>
+      <c r="P102">
+        <v>15</v>
+      </c>
+      <c r="Q102">
+        <v>6.2615800000000004</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>18</v>
       </c>
@@ -3279,8 +4545,32 @@
       <c r="H103">
         <v>4.1666699999999999</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J103" t="s">
+        <v>43</v>
+      </c>
+      <c r="K103" t="s">
+        <v>12</v>
+      </c>
+      <c r="L103">
+        <v>5000</v>
+      </c>
+      <c r="M103">
+        <v>784</v>
+      </c>
+      <c r="N103">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O103">
+        <v>2301</v>
+      </c>
+      <c r="P103">
+        <v>10</v>
+      </c>
+      <c r="Q103">
+        <v>2.4083000000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>18</v>
       </c>
@@ -3305,8 +4595,32 @@
       <c r="H104">
         <v>5.7823099999999998</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J104" t="s">
+        <v>43</v>
+      </c>
+      <c r="K104" t="s">
+        <v>12</v>
+      </c>
+      <c r="L104">
+        <v>5000</v>
+      </c>
+      <c r="M104">
+        <v>784</v>
+      </c>
+      <c r="N104">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O104">
+        <v>2301</v>
+      </c>
+      <c r="P104">
+        <v>5</v>
+      </c>
+      <c r="Q104">
+        <v>2.2971499999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>18</v>
       </c>
@@ -3331,8 +4645,32 @@
       <c r="H105">
         <v>32.113039999999998</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J105" t="s">
+        <v>43</v>
+      </c>
+      <c r="K105" t="s">
+        <v>12</v>
+      </c>
+      <c r="L105">
+        <v>5000</v>
+      </c>
+      <c r="M105">
+        <v>784</v>
+      </c>
+      <c r="N105">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O105">
+        <v>2301</v>
+      </c>
+      <c r="P105">
+        <v>1</v>
+      </c>
+      <c r="Q105">
+        <v>2.9270100000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>18</v>
       </c>
@@ -3357,8 +4695,32 @@
       <c r="H106">
         <v>30.89274</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J106" t="s">
+        <v>44</v>
+      </c>
+      <c r="K106" t="s">
+        <v>8</v>
+      </c>
+      <c r="L106">
+        <v>10000</v>
+      </c>
+      <c r="M106">
+        <v>784</v>
+      </c>
+      <c r="N106">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O106">
+        <v>6732</v>
+      </c>
+      <c r="P106">
+        <v>45</v>
+      </c>
+      <c r="Q106">
+        <v>1.8971800000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>18</v>
       </c>
@@ -3383,8 +4745,32 @@
       <c r="H107">
         <v>27.167629999999999</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J107" t="s">
+        <v>44</v>
+      </c>
+      <c r="K107" t="s">
+        <v>8</v>
+      </c>
+      <c r="L107">
+        <v>10000</v>
+      </c>
+      <c r="M107">
+        <v>784</v>
+      </c>
+      <c r="N107">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O107">
+        <v>6732</v>
+      </c>
+      <c r="P107">
+        <v>40</v>
+      </c>
+      <c r="Q107">
+        <v>1.7441899999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>18</v>
       </c>
@@ -3409,8 +4795,32 @@
       <c r="H108">
         <v>24.85549</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J108" t="s">
+        <v>44</v>
+      </c>
+      <c r="K108" t="s">
+        <v>8</v>
+      </c>
+      <c r="L108">
+        <v>10000</v>
+      </c>
+      <c r="M108">
+        <v>784</v>
+      </c>
+      <c r="N108">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O108">
+        <v>6732</v>
+      </c>
+      <c r="P108">
+        <v>35</v>
+      </c>
+      <c r="Q108">
+        <v>1.6217900000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>18</v>
       </c>
@@ -3435,8 +4845,32 @@
       <c r="H109">
         <v>20.680800000000001</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J109" t="s">
+        <v>44</v>
+      </c>
+      <c r="K109" t="s">
+        <v>8</v>
+      </c>
+      <c r="L109">
+        <v>10000</v>
+      </c>
+      <c r="M109">
+        <v>784</v>
+      </c>
+      <c r="N109">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O109">
+        <v>6732</v>
+      </c>
+      <c r="P109">
+        <v>30</v>
+      </c>
+      <c r="Q109">
+        <v>1.34639</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>18</v>
       </c>
@@ -3461,8 +4895,32 @@
       <c r="H110">
         <v>14.32241</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J110" t="s">
+        <v>44</v>
+      </c>
+      <c r="K110" t="s">
+        <v>8</v>
+      </c>
+      <c r="L110">
+        <v>10000</v>
+      </c>
+      <c r="M110">
+        <v>784</v>
+      </c>
+      <c r="N110">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O110">
+        <v>6732</v>
+      </c>
+      <c r="P110">
+        <v>25</v>
+      </c>
+      <c r="Q110">
+        <v>1.13219</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>18</v>
       </c>
@@ -3487,8 +4945,32 @@
       <c r="H111">
         <v>10.918430000000001</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J111" t="s">
+        <v>44</v>
+      </c>
+      <c r="K111" t="s">
+        <v>8</v>
+      </c>
+      <c r="L111">
+        <v>10000</v>
+      </c>
+      <c r="M111">
+        <v>784</v>
+      </c>
+      <c r="N111">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O111">
+        <v>6732</v>
+      </c>
+      <c r="P111">
+        <v>20</v>
+      </c>
+      <c r="Q111">
+        <v>1.0403899999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>18</v>
       </c>
@@ -3513,8 +4995,32 @@
       <c r="H112">
         <v>9.6981400000000004</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J112" t="s">
+        <v>44</v>
+      </c>
+      <c r="K112" t="s">
+        <v>8</v>
+      </c>
+      <c r="L112">
+        <v>10000</v>
+      </c>
+      <c r="M112">
+        <v>784</v>
+      </c>
+      <c r="N112">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O112">
+        <v>6732</v>
+      </c>
+      <c r="P112">
+        <v>15</v>
+      </c>
+      <c r="Q112">
+        <v>0.88739000000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>18</v>
       </c>
@@ -3539,8 +5045,32 @@
       <c r="H113">
         <v>8.4778400000000005</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J113" t="s">
+        <v>44</v>
+      </c>
+      <c r="K113" t="s">
+        <v>8</v>
+      </c>
+      <c r="L113">
+        <v>10000</v>
+      </c>
+      <c r="M113">
+        <v>784</v>
+      </c>
+      <c r="N113">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O113">
+        <v>6732</v>
+      </c>
+      <c r="P113">
+        <v>10</v>
+      </c>
+      <c r="Q113">
+        <v>0.70379000000000003</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>18</v>
       </c>
@@ -3565,8 +5095,32 @@
       <c r="H114">
         <v>12.0745</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J114" t="s">
+        <v>44</v>
+      </c>
+      <c r="K114" t="s">
+        <v>8</v>
+      </c>
+      <c r="L114">
+        <v>10000</v>
+      </c>
+      <c r="M114">
+        <v>784</v>
+      </c>
+      <c r="N114">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O114">
+        <v>6732</v>
+      </c>
+      <c r="P114">
+        <v>5</v>
+      </c>
+      <c r="Q114">
+        <v>0.76498999999999995</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -3591,8 +5145,32 @@
       <c r="H115">
         <v>33.396949999999997</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J115" t="s">
+        <v>44</v>
+      </c>
+      <c r="K115" t="s">
+        <v>8</v>
+      </c>
+      <c r="L115">
+        <v>10000</v>
+      </c>
+      <c r="M115">
+        <v>784</v>
+      </c>
+      <c r="N115">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O115">
+        <v>6732</v>
+      </c>
+      <c r="P115">
+        <v>1</v>
+      </c>
+      <c r="Q115">
+        <v>0.5202</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>18</v>
       </c>
@@ -3617,8 +5195,32 @@
       <c r="H116">
         <v>32.951650000000001</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J116" t="s">
+        <v>44</v>
+      </c>
+      <c r="K116" t="s">
+        <v>12</v>
+      </c>
+      <c r="L116">
+        <v>10000</v>
+      </c>
+      <c r="M116">
+        <v>784</v>
+      </c>
+      <c r="N116">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O116">
+        <v>4609</v>
+      </c>
+      <c r="P116">
+        <v>45</v>
+      </c>
+      <c r="Q116">
+        <v>11.05546</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>18</v>
       </c>
@@ -3643,8 +5245,32 @@
       <c r="H117">
         <v>31.99746</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J117" t="s">
+        <v>44</v>
+      </c>
+      <c r="K117" t="s">
+        <v>12</v>
+      </c>
+      <c r="L117">
+        <v>10000</v>
+      </c>
+      <c r="M117">
+        <v>784</v>
+      </c>
+      <c r="N117">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O117">
+        <v>4609</v>
+      </c>
+      <c r="P117">
+        <v>40</v>
+      </c>
+      <c r="Q117">
+        <v>7.9762599999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -3669,8 +5295,32 @@
       <c r="H118">
         <v>28.816790000000001</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J118" t="s">
+        <v>44</v>
+      </c>
+      <c r="K118" t="s">
+        <v>12</v>
+      </c>
+      <c r="L118">
+        <v>10000</v>
+      </c>
+      <c r="M118">
+        <v>784</v>
+      </c>
+      <c r="N118">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O118">
+        <v>4609</v>
+      </c>
+      <c r="P118">
+        <v>35</v>
+      </c>
+      <c r="Q118">
+        <v>5.6575800000000003</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>18</v>
       </c>
@@ -3695,8 +5345,32 @@
       <c r="H119">
         <v>23.473279999999999</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J119" t="s">
+        <v>44</v>
+      </c>
+      <c r="K119" t="s">
+        <v>12</v>
+      </c>
+      <c r="L119">
+        <v>10000</v>
+      </c>
+      <c r="M119">
+        <v>784</v>
+      </c>
+      <c r="N119">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O119">
+        <v>4609</v>
+      </c>
+      <c r="P119">
+        <v>30</v>
+      </c>
+      <c r="Q119">
+        <v>4.13652</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>18</v>
       </c>
@@ -3721,8 +5395,32 @@
       <c r="H120">
         <v>18.95674</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J120" t="s">
+        <v>44</v>
+      </c>
+      <c r="K120" t="s">
+        <v>12</v>
+      </c>
+      <c r="L120">
+        <v>10000</v>
+      </c>
+      <c r="M120">
+        <v>784</v>
+      </c>
+      <c r="N120">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O120">
+        <v>4609</v>
+      </c>
+      <c r="P120">
+        <v>25</v>
+      </c>
+      <c r="Q120">
+        <v>3.4316499999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>18</v>
       </c>
@@ -3747,8 +5445,32 @@
       <c r="H121">
         <v>15.585240000000001</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J121" t="s">
+        <v>44</v>
+      </c>
+      <c r="K121" t="s">
+        <v>12</v>
+      </c>
+      <c r="L121">
+        <v>10000</v>
+      </c>
+      <c r="M121">
+        <v>784</v>
+      </c>
+      <c r="N121">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O121">
+        <v>4609</v>
+      </c>
+      <c r="P121">
+        <v>20</v>
+      </c>
+      <c r="Q121">
+        <v>3.0235599999999998</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -3773,8 +5495,32 @@
       <c r="H122">
         <v>12.78626</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J122" t="s">
+        <v>44</v>
+      </c>
+      <c r="K122" t="s">
+        <v>12</v>
+      </c>
+      <c r="L122">
+        <v>10000</v>
+      </c>
+      <c r="M122">
+        <v>784</v>
+      </c>
+      <c r="N122">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O122">
+        <v>4609</v>
+      </c>
+      <c r="P122">
+        <v>15</v>
+      </c>
+      <c r="Q122">
+        <v>2.3001299999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>18</v>
       </c>
@@ -3799,8 +5545,32 @@
       <c r="H123">
         <v>8.58779</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J123" t="s">
+        <v>44</v>
+      </c>
+      <c r="K123" t="s">
+        <v>12</v>
+      </c>
+      <c r="L123">
+        <v>10000</v>
+      </c>
+      <c r="M123">
+        <v>784</v>
+      </c>
+      <c r="N123">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O123">
+        <v>4609</v>
+      </c>
+      <c r="P123">
+        <v>10</v>
+      </c>
+      <c r="Q123">
+        <v>1.83639</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>18</v>
       </c>
@@ -3825,8 +5595,32 @@
       <c r="H124">
         <v>11.195930000000001</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J124" t="s">
+        <v>44</v>
+      </c>
+      <c r="K124" t="s">
+        <v>12</v>
+      </c>
+      <c r="L124">
+        <v>10000</v>
+      </c>
+      <c r="M124">
+        <v>784</v>
+      </c>
+      <c r="N124">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O124">
+        <v>4609</v>
+      </c>
+      <c r="P124">
+        <v>5</v>
+      </c>
+      <c r="Q124">
+        <v>1.7436499999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>18</v>
       </c>
@@ -3851,8 +5645,32 @@
       <c r="H125">
         <v>25.12171</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J125" t="s">
+        <v>44</v>
+      </c>
+      <c r="K125" t="s">
+        <v>12</v>
+      </c>
+      <c r="L125">
+        <v>10000</v>
+      </c>
+      <c r="M125">
+        <v>784</v>
+      </c>
+      <c r="N125">
+        <v>3.9477799999999998</v>
+      </c>
+      <c r="O125">
+        <v>4609</v>
+      </c>
+      <c r="P125">
+        <v>1</v>
+      </c>
+      <c r="Q125">
+        <v>1.9291400000000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>18</v>
       </c>
@@ -3877,8 +5695,32 @@
       <c r="H126">
         <v>24.537489999999998</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J126" t="s">
+        <v>43</v>
+      </c>
+      <c r="K126" t="s">
+        <v>32</v>
+      </c>
+      <c r="L126">
+        <v>5000</v>
+      </c>
+      <c r="M126">
+        <v>784</v>
+      </c>
+      <c r="N126">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O126">
+        <v>3383</v>
+      </c>
+      <c r="P126">
+        <v>45</v>
+      </c>
+      <c r="Q126">
+        <v>6.1842899999999998</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>18</v>
       </c>
@@ -3903,8 +5745,32 @@
       <c r="H127">
         <v>22.687439999999999</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J127" t="s">
+        <v>43</v>
+      </c>
+      <c r="K127" t="s">
+        <v>32</v>
+      </c>
+      <c r="L127">
+        <v>5000</v>
+      </c>
+      <c r="M127">
+        <v>784</v>
+      </c>
+      <c r="N127">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O127">
+        <v>3383</v>
+      </c>
+      <c r="P127">
+        <v>40</v>
+      </c>
+      <c r="Q127">
+        <v>5.8750799999999996</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>18</v>
       </c>
@@ -3929,8 +5795,32 @@
       <c r="H128">
         <v>22.395330000000001</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J128" t="s">
+        <v>43</v>
+      </c>
+      <c r="K128" t="s">
+        <v>32</v>
+      </c>
+      <c r="L128">
+        <v>5000</v>
+      </c>
+      <c r="M128">
+        <v>784</v>
+      </c>
+      <c r="N128">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O128">
+        <v>3383</v>
+      </c>
+      <c r="P128">
+        <v>35</v>
+      </c>
+      <c r="Q128">
+        <v>5.6895499999999997</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>18</v>
       </c>
@@ -3955,8 +5845,32 @@
       <c r="H129">
         <v>18.695229999999999</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J129" t="s">
+        <v>43</v>
+      </c>
+      <c r="K129" t="s">
+        <v>32</v>
+      </c>
+      <c r="L129">
+        <v>5000</v>
+      </c>
+      <c r="M129">
+        <v>784</v>
+      </c>
+      <c r="N129">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O129">
+        <v>3383</v>
+      </c>
+      <c r="P129">
+        <v>30</v>
+      </c>
+      <c r="Q129">
+        <v>5.0092800000000004</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>18</v>
       </c>
@@ -3981,8 +5895,32 @@
       <c r="H130">
         <v>15.092499999999999</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J130" t="s">
+        <v>43</v>
+      </c>
+      <c r="K130" t="s">
+        <v>32</v>
+      </c>
+      <c r="L130">
+        <v>5000</v>
+      </c>
+      <c r="M130">
+        <v>784</v>
+      </c>
+      <c r="N130">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O130">
+        <v>3383</v>
+      </c>
+      <c r="P130">
+        <v>25</v>
+      </c>
+      <c r="Q130">
+        <v>4.9474299999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -4007,8 +5945,32 @@
       <c r="H131">
         <v>12.755599999999999</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J131" t="s">
+        <v>43</v>
+      </c>
+      <c r="K131" t="s">
+        <v>32</v>
+      </c>
+      <c r="L131">
+        <v>5000</v>
+      </c>
+      <c r="M131">
+        <v>784</v>
+      </c>
+      <c r="N131">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O131">
+        <v>3383</v>
+      </c>
+      <c r="P131">
+        <v>20</v>
+      </c>
+      <c r="Q131">
+        <v>4.5145299999999997</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>18</v>
       </c>
@@ -4033,8 +5995,32 @@
       <c r="H132">
         <v>12.17137</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J132" t="s">
+        <v>43</v>
+      </c>
+      <c r="K132" t="s">
+        <v>32</v>
+      </c>
+      <c r="L132">
+        <v>5000</v>
+      </c>
+      <c r="M132">
+        <v>784</v>
+      </c>
+      <c r="N132">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O132">
+        <v>3383</v>
+      </c>
+      <c r="P132">
+        <v>15</v>
+      </c>
+      <c r="Q132">
+        <v>4.1434800000000003</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>18</v>
       </c>
@@ -4059,8 +6045,32 @@
       <c r="H133">
         <v>6.7186000000000003</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J133" t="s">
+        <v>43</v>
+      </c>
+      <c r="K133" t="s">
+        <v>32</v>
+      </c>
+      <c r="L133">
+        <v>5000</v>
+      </c>
+      <c r="M133">
+        <v>784</v>
+      </c>
+      <c r="N133">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O133">
+        <v>3383</v>
+      </c>
+      <c r="P133">
+        <v>10</v>
+      </c>
+      <c r="Q133">
+        <v>3.7105800000000002</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>18</v>
       </c>
@@ -4085,8 +6095,32 @@
       <c r="H134">
         <v>4.1869500000000004</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J134" t="s">
+        <v>43</v>
+      </c>
+      <c r="K134" t="s">
+        <v>32</v>
+      </c>
+      <c r="L134">
+        <v>5000</v>
+      </c>
+      <c r="M134">
+        <v>784</v>
+      </c>
+      <c r="N134">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O134">
+        <v>3383</v>
+      </c>
+      <c r="P134">
+        <v>5</v>
+      </c>
+      <c r="Q134">
+        <v>3.8961000000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -4111,8 +6145,32 @@
       <c r="H135">
         <v>35.457920000000001</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J135" t="s">
+        <v>43</v>
+      </c>
+      <c r="K135" t="s">
+        <v>32</v>
+      </c>
+      <c r="L135">
+        <v>5000</v>
+      </c>
+      <c r="M135">
+        <v>784</v>
+      </c>
+      <c r="N135">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O135">
+        <v>3383</v>
+      </c>
+      <c r="P135">
+        <v>1</v>
+      </c>
+      <c r="Q135">
+        <v>3.83426</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>18</v>
       </c>
@@ -4137,8 +6195,32 @@
       <c r="H136">
         <v>34.405940000000001</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J136" t="s">
+        <v>43</v>
+      </c>
+      <c r="K136" t="s">
+        <v>32</v>
+      </c>
+      <c r="L136">
+        <v>5000</v>
+      </c>
+      <c r="M136">
+        <v>784</v>
+      </c>
+      <c r="N136">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O136">
+        <v>2301</v>
+      </c>
+      <c r="P136">
+        <v>45</v>
+      </c>
+      <c r="Q136">
+        <v>9.2997399999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>18</v>
       </c>
@@ -4163,8 +6245,32 @@
       <c r="H137">
         <v>33.353960000000001</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J137" t="s">
+        <v>43</v>
+      </c>
+      <c r="K137" t="s">
+        <v>32</v>
+      </c>
+      <c r="L137">
+        <v>5000</v>
+      </c>
+      <c r="M137">
+        <v>784</v>
+      </c>
+      <c r="N137">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O137">
+        <v>2301</v>
+      </c>
+      <c r="P137">
+        <v>40</v>
+      </c>
+      <c r="Q137">
+        <v>9.1885899999999996</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>18</v>
       </c>
@@ -4189,8 +6295,32 @@
       <c r="H138">
         <v>31.745049999999999</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J138" t="s">
+        <v>43</v>
+      </c>
+      <c r="K138" t="s">
+        <v>32</v>
+      </c>
+      <c r="L138">
+        <v>5000</v>
+      </c>
+      <c r="M138">
+        <v>784</v>
+      </c>
+      <c r="N138">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O138">
+        <v>2301</v>
+      </c>
+      <c r="P138">
+        <v>35</v>
+      </c>
+      <c r="Q138">
+        <v>8.2993699999999997</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>18</v>
       </c>
@@ -4215,8 +6345,32 @@
       <c r="H139">
         <v>27.59901</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J139" t="s">
+        <v>43</v>
+      </c>
+      <c r="K139" t="s">
+        <v>32</v>
+      </c>
+      <c r="L139">
+        <v>5000</v>
+      </c>
+      <c r="M139">
+        <v>784</v>
+      </c>
+      <c r="N139">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O139">
+        <v>2301</v>
+      </c>
+      <c r="P139">
+        <v>30</v>
+      </c>
+      <c r="Q139">
+        <v>7.5213000000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>18</v>
       </c>
@@ -4241,8 +6395,32 @@
       <c r="H140">
         <v>23.0198</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J140" t="s">
+        <v>43</v>
+      </c>
+      <c r="K140" t="s">
+        <v>32</v>
+      </c>
+      <c r="L140">
+        <v>5000</v>
+      </c>
+      <c r="M140">
+        <v>784</v>
+      </c>
+      <c r="N140">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O140">
+        <v>2301</v>
+      </c>
+      <c r="P140">
+        <v>25</v>
+      </c>
+      <c r="Q140">
+        <v>7.0396400000000003</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>18</v>
       </c>
@@ -4267,8 +6445,32 @@
       <c r="H141">
         <v>17.574259999999999</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J141" t="s">
+        <v>43</v>
+      </c>
+      <c r="K141" t="s">
+        <v>32</v>
+      </c>
+      <c r="L141">
+        <v>5000</v>
+      </c>
+      <c r="M141">
+        <v>784</v>
+      </c>
+      <c r="N141">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O141">
+        <v>2301</v>
+      </c>
+      <c r="P141">
+        <v>20</v>
+      </c>
+      <c r="Q141">
+        <v>6.7432400000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>18</v>
       </c>
@@ -4293,8 +6495,32 @@
       <c r="H142">
         <v>12.06683</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J142" t="s">
+        <v>43</v>
+      </c>
+      <c r="K142" t="s">
+        <v>32</v>
+      </c>
+      <c r="L142">
+        <v>5000</v>
+      </c>
+      <c r="M142">
+        <v>784</v>
+      </c>
+      <c r="N142">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O142">
+        <v>2301</v>
+      </c>
+      <c r="P142">
+        <v>15</v>
+      </c>
+      <c r="Q142">
+        <v>5.8540200000000002</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>18</v>
       </c>
@@ -4319,8 +6545,32 @@
       <c r="H143">
         <v>12.623760000000001</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J143" t="s">
+        <v>43</v>
+      </c>
+      <c r="K143" t="s">
+        <v>32</v>
+      </c>
+      <c r="L143">
+        <v>5000</v>
+      </c>
+      <c r="M143">
+        <v>784</v>
+      </c>
+      <c r="N143">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O143">
+        <v>2301</v>
+      </c>
+      <c r="P143">
+        <v>10</v>
+      </c>
+      <c r="Q143">
+        <v>5.2241600000000004</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -4345,8 +6595,32 @@
       <c r="H144">
         <v>11.324260000000001</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J144" t="s">
+        <v>43</v>
+      </c>
+      <c r="K144" t="s">
+        <v>32</v>
+      </c>
+      <c r="L144">
+        <v>5000</v>
+      </c>
+      <c r="M144">
+        <v>784</v>
+      </c>
+      <c r="N144">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O144">
+        <v>2301</v>
+      </c>
+      <c r="P144">
+        <v>5</v>
+      </c>
+      <c r="Q144">
+        <v>4.7054499999999999</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>18</v>
       </c>
@@ -4371,8 +6645,32 @@
       <c r="H145">
         <v>50.662979999999997</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J145" t="s">
+        <v>43</v>
+      </c>
+      <c r="K145" t="s">
+        <v>32</v>
+      </c>
+      <c r="L145">
+        <v>5000</v>
+      </c>
+      <c r="M145">
+        <v>784</v>
+      </c>
+      <c r="N145">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O145">
+        <v>2301</v>
+      </c>
+      <c r="P145">
+        <v>1</v>
+      </c>
+      <c r="Q145">
+        <v>4.3719900000000003</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>18</v>
       </c>
@@ -4397,8 +6695,32 @@
       <c r="H146">
         <v>47.403309999999998</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J146" t="s">
+        <v>44</v>
+      </c>
+      <c r="K146" t="s">
+        <v>32</v>
+      </c>
+      <c r="L146">
+        <v>10000</v>
+      </c>
+      <c r="M146">
+        <v>784</v>
+      </c>
+      <c r="N146">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O146">
+        <v>6732</v>
+      </c>
+      <c r="P146">
+        <v>45</v>
+      </c>
+      <c r="Q146">
+        <v>6.7931499999999998</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>18</v>
       </c>
@@ -4423,8 +6745,32 @@
       <c r="H147">
         <v>45.027619999999999</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J147" t="s">
+        <v>44</v>
+      </c>
+      <c r="K147" t="s">
+        <v>32</v>
+      </c>
+      <c r="L147">
+        <v>10000</v>
+      </c>
+      <c r="M147">
+        <v>784</v>
+      </c>
+      <c r="N147">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O147">
+        <v>6732</v>
+      </c>
+      <c r="P147">
+        <v>40</v>
+      </c>
+      <c r="Q147">
+        <v>6.6095499999999996</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>18</v>
       </c>
@@ -4449,8 +6795,32 @@
       <c r="H148">
         <v>42.209940000000003</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J148" t="s">
+        <v>44</v>
+      </c>
+      <c r="K148" t="s">
+        <v>32</v>
+      </c>
+      <c r="L148">
+        <v>10000</v>
+      </c>
+      <c r="M148">
+        <v>784</v>
+      </c>
+      <c r="N148">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O148">
+        <v>6732</v>
+      </c>
+      <c r="P148">
+        <v>35</v>
+      </c>
+      <c r="Q148">
+        <v>6.1811499999999997</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>18</v>
       </c>
@@ -4475,8 +6845,32 @@
       <c r="H149">
         <v>39.558010000000003</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J149" t="s">
+        <v>44</v>
+      </c>
+      <c r="K149" t="s">
+        <v>32</v>
+      </c>
+      <c r="L149">
+        <v>10000</v>
+      </c>
+      <c r="M149">
+        <v>784</v>
+      </c>
+      <c r="N149">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O149">
+        <v>6732</v>
+      </c>
+      <c r="P149">
+        <v>30</v>
+      </c>
+      <c r="Q149">
+        <v>5.93635</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>18</v>
       </c>
@@ -4501,8 +6895,32 @@
       <c r="H150">
         <v>37.127070000000003</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J150" t="s">
+        <v>44</v>
+      </c>
+      <c r="K150" t="s">
+        <v>32</v>
+      </c>
+      <c r="L150">
+        <v>10000</v>
+      </c>
+      <c r="M150">
+        <v>784</v>
+      </c>
+      <c r="N150">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O150">
+        <v>6732</v>
+      </c>
+      <c r="P150">
+        <v>25</v>
+      </c>
+      <c r="Q150">
+        <v>5.47736</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>18</v>
       </c>
@@ -4527,8 +6945,32 @@
       <c r="H151">
         <v>33.922649999999997</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J151" t="s">
+        <v>44</v>
+      </c>
+      <c r="K151" t="s">
+        <v>32</v>
+      </c>
+      <c r="L151">
+        <v>10000</v>
+      </c>
+      <c r="M151">
+        <v>784</v>
+      </c>
+      <c r="N151">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O151">
+        <v>6732</v>
+      </c>
+      <c r="P151">
+        <v>20</v>
+      </c>
+      <c r="Q151">
+        <v>4.8959599999999996</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>18</v>
       </c>
@@ -4553,8 +6995,32 @@
       <c r="H152">
         <v>26.187850000000001</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J152" t="s">
+        <v>44</v>
+      </c>
+      <c r="K152" t="s">
+        <v>32</v>
+      </c>
+      <c r="L152">
+        <v>10000</v>
+      </c>
+      <c r="M152">
+        <v>784</v>
+      </c>
+      <c r="N152">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O152">
+        <v>6732</v>
+      </c>
+      <c r="P152">
+        <v>15</v>
+      </c>
+      <c r="Q152">
+        <v>4.4063600000000003</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>18</v>
       </c>
@@ -4579,8 +7045,32 @@
       <c r="H153">
         <v>21.43646</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J153" t="s">
+        <v>44</v>
+      </c>
+      <c r="K153" t="s">
+        <v>32</v>
+      </c>
+      <c r="L153">
+        <v>10000</v>
+      </c>
+      <c r="M153">
+        <v>784</v>
+      </c>
+      <c r="N153">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O153">
+        <v>6732</v>
+      </c>
+      <c r="P153">
+        <v>10</v>
+      </c>
+      <c r="Q153">
+        <v>3.9167700000000001</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>18</v>
       </c>
@@ -4605,8 +7095,32 @@
       <c r="H154">
         <v>19.39227</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J154" t="s">
+        <v>44</v>
+      </c>
+      <c r="K154" t="s">
+        <v>32</v>
+      </c>
+      <c r="L154">
+        <v>10000</v>
+      </c>
+      <c r="M154">
+        <v>784</v>
+      </c>
+      <c r="N154">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O154">
+        <v>6732</v>
+      </c>
+      <c r="P154">
+        <v>5</v>
+      </c>
+      <c r="Q154">
+        <v>3.7025700000000001</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>18</v>
       </c>
@@ -4631,8 +7145,32 @@
       <c r="H155">
         <v>48.5351</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J155" t="s">
+        <v>44</v>
+      </c>
+      <c r="K155" t="s">
+        <v>32</v>
+      </c>
+      <c r="L155">
+        <v>10000</v>
+      </c>
+      <c r="M155">
+        <v>784</v>
+      </c>
+      <c r="N155">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O155">
+        <v>6732</v>
+      </c>
+      <c r="P155">
+        <v>1</v>
+      </c>
+      <c r="Q155">
+        <v>3.3965700000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>18</v>
       </c>
@@ -4657,8 +7195,32 @@
       <c r="H156">
         <v>45.771140000000003</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J156" t="s">
+        <v>44</v>
+      </c>
+      <c r="K156" t="s">
+        <v>32</v>
+      </c>
+      <c r="L156">
+        <v>10000</v>
+      </c>
+      <c r="M156">
+        <v>784</v>
+      </c>
+      <c r="N156">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O156">
+        <v>4609</v>
+      </c>
+      <c r="P156">
+        <v>45</v>
+      </c>
+      <c r="Q156">
+        <v>6.3624599999999996</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>18</v>
       </c>
@@ -4683,8 +7245,32 @@
       <c r="H157">
         <v>42.786070000000002</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J157" t="s">
+        <v>44</v>
+      </c>
+      <c r="K157" t="s">
+        <v>32</v>
+      </c>
+      <c r="L157">
+        <v>10000</v>
+      </c>
+      <c r="M157">
+        <v>784</v>
+      </c>
+      <c r="N157">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O157">
+        <v>4609</v>
+      </c>
+      <c r="P157">
+        <v>40</v>
+      </c>
+      <c r="Q157">
+        <v>6.1955099999999996</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>18</v>
       </c>
@@ -4709,8 +7295,32 @@
       <c r="H158">
         <v>41.127690000000001</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J158" t="s">
+        <v>44</v>
+      </c>
+      <c r="K158" t="s">
+        <v>32</v>
+      </c>
+      <c r="L158">
+        <v>10000</v>
+      </c>
+      <c r="M158">
+        <v>784</v>
+      </c>
+      <c r="N158">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O158">
+        <v>4609</v>
+      </c>
+      <c r="P158">
+        <v>35</v>
+      </c>
+      <c r="Q158">
+        <v>5.8801699999999997</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>18</v>
       </c>
@@ -4735,8 +7345,32 @@
       <c r="H159">
         <v>39.248199999999997</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J159" t="s">
+        <v>44</v>
+      </c>
+      <c r="K159" t="s">
+        <v>32</v>
+      </c>
+      <c r="L159">
+        <v>10000</v>
+      </c>
+      <c r="M159">
+        <v>784</v>
+      </c>
+      <c r="N159">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O159">
+        <v>4609</v>
+      </c>
+      <c r="P159">
+        <v>30</v>
+      </c>
+      <c r="Q159">
+        <v>5.58338</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>18</v>
       </c>
@@ -4761,8 +7395,32 @@
       <c r="H160">
         <v>36.097290000000001</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J160" t="s">
+        <v>44</v>
+      </c>
+      <c r="K160" t="s">
+        <v>32</v>
+      </c>
+      <c r="L160">
+        <v>10000</v>
+      </c>
+      <c r="M160">
+        <v>784</v>
+      </c>
+      <c r="N160">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O160">
+        <v>4609</v>
+      </c>
+      <c r="P160">
+        <v>25</v>
+      </c>
+      <c r="Q160">
+        <v>5.4349800000000004</v>
+      </c>
+    </row>
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>18</v>
       </c>
@@ -4787,8 +7445,32 @@
       <c r="H161">
         <v>32.669980000000002</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J161" t="s">
+        <v>44</v>
+      </c>
+      <c r="K161" t="s">
+        <v>32</v>
+      </c>
+      <c r="L161">
+        <v>10000</v>
+      </c>
+      <c r="M161">
+        <v>784</v>
+      </c>
+      <c r="N161">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O161">
+        <v>4609</v>
+      </c>
+      <c r="P161">
+        <v>20</v>
+      </c>
+      <c r="Q161">
+        <v>4.9341499999999998</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>18</v>
       </c>
@@ -4813,8 +7495,32 @@
       <c r="H162">
         <v>23.10669</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J162" t="s">
+        <v>44</v>
+      </c>
+      <c r="K162" t="s">
+        <v>32</v>
+      </c>
+      <c r="L162">
+        <v>10000</v>
+      </c>
+      <c r="M162">
+        <v>784</v>
+      </c>
+      <c r="N162">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O162">
+        <v>4609</v>
+      </c>
+      <c r="P162">
+        <v>15</v>
+      </c>
+      <c r="Q162">
+        <v>4.7115600000000004</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>18</v>
       </c>
@@ -4839,8 +7545,32 @@
       <c r="H163">
         <v>22.498619999999999</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J163" t="s">
+        <v>44</v>
+      </c>
+      <c r="K163" t="s">
+        <v>32</v>
+      </c>
+      <c r="L163">
+        <v>10000</v>
+      </c>
+      <c r="M163">
+        <v>784</v>
+      </c>
+      <c r="N163">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O163">
+        <v>4609</v>
+      </c>
+      <c r="P163">
+        <v>10</v>
+      </c>
+      <c r="Q163">
+        <v>4.2663700000000002</v>
+      </c>
+    </row>
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>18</v>
       </c>
@@ -4865,10 +7595,62 @@
       <c r="H164">
         <v>19.568819999999999</v>
       </c>
+      <c r="J164" t="s">
+        <v>44</v>
+      </c>
+      <c r="K164" t="s">
+        <v>32</v>
+      </c>
+      <c r="L164">
+        <v>10000</v>
+      </c>
+      <c r="M164">
+        <v>784</v>
+      </c>
+      <c r="N164">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O164">
+        <v>4609</v>
+      </c>
+      <c r="P164">
+        <v>5</v>
+      </c>
+      <c r="Q164">
+        <v>4.0623300000000002</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J165" t="s">
+        <v>44</v>
+      </c>
+      <c r="K165" t="s">
+        <v>32</v>
+      </c>
+      <c r="L165">
+        <v>10000</v>
+      </c>
+      <c r="M165">
+        <v>784</v>
+      </c>
+      <c r="N165">
+        <v>4.1203200000000004</v>
+      </c>
+      <c r="O165">
+        <v>4609</v>
+      </c>
+      <c r="P165">
+        <v>1</v>
+      </c>
+      <c r="Q165">
+        <v>3.9139300000000001</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I25:O25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- generated compression results for SAT_Results_2012 - tried active learning based kNN classification for larger MNIST subsets - visualized the distribution of #points requiring an atom for their reconstruction for dp-max and dp-mean for SAT_Results_2012
</commit_message>
<xml_diff>
--- a/output/to_publish/results12.xlsx
+++ b/output/to_publish/results12.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="55">
   <si>
     <t>Dataset</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>variable sparsity+maj vote</t>
-  </si>
-  <si>
-    <t>mnist2-deskewed - #points = 2000</t>
   </si>
   <si>
     <t>dp-max (1361)</t>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>randomized (4609)</t>
+  </si>
+  <si>
+    <t>variable sparsity+weighted kNN(on atoms)</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1097,7 @@
   <dimension ref="A1:Q165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P50" sqref="P50"/>
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,7 +1118,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -1127,7 +1127,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="I1" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="5">
         <v>45</v>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="5">
         <v>45</v>
@@ -1197,7 +1197,7 @@
         <v>11.11111</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" s="5">
         <v>45</v>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="L3" s="5"/>
       <c r="M3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N3" s="5">
         <v>45</v>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="5">
         <v>40</v>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4" s="5">
         <v>40</v>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="5">
         <v>35</v>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N5" s="5">
         <v>35</v>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="5">
         <v>30</v>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N6" s="5">
         <v>30</v>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="5">
         <v>25</v>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N7" s="5">
         <v>25</v>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="5">
         <v>20</v>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N8" s="5">
         <v>20</v>
@@ -1428,7 +1428,7 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="5">
         <v>15</v>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N9" s="5">
         <v>15</v>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="5">
         <v>10</v>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N10" s="5">
         <v>10</v>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="5">
         <v>5</v>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N11" s="5">
         <v>5</v>
@@ -1548,7 +1548,7 @@
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N12" s="5">
         <v>1</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="5">
         <v>45</v>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="5">
         <v>45</v>
@@ -1597,7 +1597,7 @@
         <v>14.455780000000001</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J13" s="5">
         <v>45</v>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N13" s="5">
         <v>45</v>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="5">
         <v>40</v>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N14" s="5">
         <v>40</v>
@@ -1668,7 +1668,7 @@
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="5">
         <v>35</v>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N15" s="5">
         <v>35</v>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="5">
         <v>30</v>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N16" s="5">
         <v>30</v>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" s="5">
         <v>25</v>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N17" s="5">
         <v>25</v>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" s="5">
         <v>20</v>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N18" s="5">
         <v>20</v>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="5">
         <v>15</v>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N19" s="5">
         <v>15</v>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="5">
         <v>10</v>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N20" s="5">
         <v>10</v>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21" s="5">
         <v>5</v>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N21" s="5">
         <v>5</v>
@@ -1948,7 +1948,7 @@
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22" s="5">
         <v>1</v>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N22" s="5">
         <v>1</v>
@@ -1978,7 +1978,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="5">
         <v>45</v>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" s="5">
         <v>45</v>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24" s="5">
         <v>40</v>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25" s="5">
         <v>35</v>
@@ -2039,7 +2039,7 @@
         <v>18.689789999999999</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F26" s="5">
         <v>30</v>
@@ -2100,7 +2100,7 @@
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27" s="5">
         <v>25</v>
@@ -2109,7 +2109,7 @@
         <v>15.221579999999999</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J27" s="5">
         <v>45</v>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N27" s="5">
         <v>45</v>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28" s="5">
         <v>20</v>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N28" s="5">
         <v>40</v>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F29" s="5">
         <v>15</v>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="L29" s="5"/>
       <c r="M29" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N29" s="5">
         <v>35</v>
@@ -2220,7 +2220,7 @@
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F30" s="5">
         <v>10</v>
@@ -2239,7 +2239,7 @@
       </c>
       <c r="L30" s="5"/>
       <c r="M30" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N30" s="5">
         <v>30</v>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F31" s="5">
         <v>5</v>
@@ -2279,7 +2279,7 @@
       </c>
       <c r="L31" s="5"/>
       <c r="M31" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N31" s="5">
         <v>25</v>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F32" s="5">
         <v>1</v>
@@ -2319,7 +2319,7 @@
       </c>
       <c r="L32" s="5"/>
       <c r="M32" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N32" s="5">
         <v>20</v>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="5">
         <v>45</v>
@@ -2340,7 +2340,7 @@
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F33" s="5">
         <v>45</v>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="L33" s="5"/>
       <c r="M33" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N33" s="5">
         <v>15</v>
@@ -2380,7 +2380,7 @@
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F34" s="5">
         <v>40</v>
@@ -2399,7 +2399,7 @@
       </c>
       <c r="L34" s="5"/>
       <c r="M34" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N34" s="5">
         <v>10</v>
@@ -2420,7 +2420,7 @@
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F35" s="5">
         <v>35</v>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="L35" s="5"/>
       <c r="M35" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N35" s="5">
         <v>5</v>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F36" s="5">
         <v>30</v>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="L36" s="5"/>
       <c r="M36" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N36" s="5">
         <v>1</v>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F37" s="5">
         <v>25</v>
@@ -2509,7 +2509,7 @@
         <v>15.458019999999999</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J37" s="5">
         <v>45</v>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="L37" s="5"/>
       <c r="M37" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N37" s="5">
         <v>45</v>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F38" s="5">
         <v>20</v>
@@ -2559,7 +2559,7 @@
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N38" s="5">
         <v>40</v>
@@ -2580,7 +2580,7 @@
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F39" s="5">
         <v>15</v>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="L39" s="5"/>
       <c r="M39" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N39" s="5">
         <v>35</v>
@@ -2620,7 +2620,7 @@
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F40" s="5">
         <v>10</v>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="L40" s="5"/>
       <c r="M40" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N40" s="5">
         <v>30</v>
@@ -2660,7 +2660,7 @@
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F41" s="5">
         <v>5</v>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="L41" s="5"/>
       <c r="M41" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N41" s="5">
         <v>25</v>
@@ -2700,7 +2700,7 @@
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F42" s="5">
         <v>1</v>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N42" s="5">
         <v>20</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B43" s="5">
         <v>45</v>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F43" s="5">
         <v>45</v>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="L43" s="5"/>
       <c r="M43" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N43" s="5">
         <v>15</v>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F44" s="5">
         <v>40</v>
@@ -2799,7 +2799,7 @@
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N44" s="5">
         <v>10</v>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F45" s="5">
         <v>35</v>
@@ -2839,7 +2839,7 @@
       </c>
       <c r="L45" s="5"/>
       <c r="M45" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N45" s="5">
         <v>5</v>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F46" s="5">
         <v>30</v>
@@ -2879,7 +2879,7 @@
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N46" s="5">
         <v>1</v>
@@ -2900,7 +2900,7 @@
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F47" s="5">
         <v>25</v>
@@ -2921,7 +2921,7 @@
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F48" s="5">
         <v>20</v>
@@ -2942,7 +2942,7 @@
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F49" s="5">
         <v>15</v>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F50" s="5">
         <v>10</v>
@@ -2984,7 +2984,7 @@
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F51" s="5">
         <v>5</v>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F52" s="5">
         <v>1</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B53" s="5">
         <v>45</v>
@@ -3026,7 +3026,7 @@
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F53" s="5">
         <v>45</v>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F54" s="5">
         <v>40</v>
@@ -3068,7 +3068,7 @@
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F55" s="5">
         <v>35</v>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F56" s="5">
         <v>30</v>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F57" s="5">
         <v>25</v>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F58" s="5">
         <v>20</v>
@@ -3152,7 +3152,7 @@
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F59" s="5">
         <v>15</v>
@@ -3173,7 +3173,7 @@
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F60" s="5">
         <v>10</v>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F61" s="5">
         <v>5</v>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F62" s="5">
         <v>1</v>
@@ -3226,7 +3226,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B63" s="5">
         <v>45</v>
@@ -3236,7 +3236,7 @@
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F63" s="5">
         <v>45</v>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F64" s="5">
         <v>40</v>
@@ -3278,7 +3278,7 @@
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F65" s="5">
         <v>35</v>
@@ -3299,7 +3299,7 @@
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F66" s="5">
         <v>30</v>
@@ -3320,7 +3320,7 @@
       </c>
       <c r="D67" s="12"/>
       <c r="E67" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F67" s="5">
         <v>25</v>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F68" s="5">
         <v>20</v>
@@ -3362,7 +3362,7 @@
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F69" s="5">
         <v>15</v>
@@ -3383,7 +3383,7 @@
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F70" s="5">
         <v>10</v>
@@ -3404,7 +3404,7 @@
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F71" s="5">
         <v>5</v>
@@ -3425,7 +3425,7 @@
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F72" s="5">
         <v>1</v>
@@ -3436,7 +3436,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B73" s="5">
         <v>45</v>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F73" s="5">
         <v>45</v>
@@ -3467,7 +3467,7 @@
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F74" s="5">
         <v>40</v>
@@ -3488,7 +3488,7 @@
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F75" s="5">
         <v>35</v>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F76" s="5">
         <v>30</v>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F77" s="5">
         <v>25</v>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F78" s="5">
         <v>20</v>
@@ -3572,7 +3572,7 @@
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F79" s="5">
         <v>15</v>
@@ -3593,7 +3593,7 @@
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F80" s="5">
         <v>10</v>
@@ -3614,7 +3614,7 @@
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F81" s="5">
         <v>5</v>
@@ -3635,7 +3635,7 @@
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F82" s="5">
         <v>1</v>
@@ -3696,7 +3696,7 @@
         <v>28.325510000000001</v>
       </c>
       <c r="J86" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K86" t="s">
         <v>8</v>
@@ -3746,7 +3746,7 @@
         <v>24.25665</v>
       </c>
       <c r="J87" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K87" t="s">
         <v>8</v>
@@ -3796,7 +3796,7 @@
         <v>20.500779999999999</v>
       </c>
       <c r="J88" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K88" t="s">
         <v>8</v>
@@ -3846,7 +3846,7 @@
         <v>16.27543</v>
       </c>
       <c r="J89" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K89" t="s">
         <v>8</v>
@@ -3896,7 +3896,7 @@
         <v>13.30203</v>
       </c>
       <c r="J90" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K90" t="s">
         <v>8</v>
@@ -3946,7 +3946,7 @@
         <v>5.3208099999999998</v>
       </c>
       <c r="J91" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K91" t="s">
         <v>8</v>
@@ -3996,7 +3996,7 @@
         <v>1.25196</v>
       </c>
       <c r="J92" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K92" t="s">
         <v>8</v>
@@ -4046,7 +4046,7 @@
         <v>0.93896999999999997</v>
       </c>
       <c r="J93" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K93" t="s">
         <v>8</v>
@@ -4096,7 +4096,7 @@
         <v>1.25196</v>
       </c>
       <c r="J94" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K94" t="s">
         <v>8</v>
@@ -4146,7 +4146,7 @@
         <v>21.59864</v>
       </c>
       <c r="J95" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K95" t="s">
         <v>8</v>
@@ -4196,7 +4196,7 @@
         <v>17.94218</v>
       </c>
       <c r="J96" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K96" t="s">
         <v>12</v>
@@ -4246,7 +4246,7 @@
         <v>15.136049999999999</v>
       </c>
       <c r="J97" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K97" t="s">
         <v>12</v>
@@ -4296,7 +4296,7 @@
         <v>11.309519999999999</v>
       </c>
       <c r="J98" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K98" t="s">
         <v>12</v>
@@ -4346,7 +4346,7 @@
         <v>8.5033999999999992</v>
       </c>
       <c r="J99" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K99" t="s">
         <v>12</v>
@@ -4396,7 +4396,7 @@
         <v>6.1224499999999997</v>
       </c>
       <c r="J100" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K100" t="s">
         <v>12</v>
@@ -4446,7 +4446,7 @@
         <v>3.4863900000000001</v>
       </c>
       <c r="J101" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K101" t="s">
         <v>12</v>
@@ -4496,7 +4496,7 @@
         <v>3.23129</v>
       </c>
       <c r="J102" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K102" t="s">
         <v>12</v>
@@ -4546,7 +4546,7 @@
         <v>4.1666699999999999</v>
       </c>
       <c r="J103" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K103" t="s">
         <v>12</v>
@@ -4596,7 +4596,7 @@
         <v>5.7823099999999998</v>
       </c>
       <c r="J104" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K104" t="s">
         <v>12</v>
@@ -4646,7 +4646,7 @@
         <v>32.113039999999998</v>
       </c>
       <c r="J105" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K105" t="s">
         <v>12</v>
@@ -4696,7 +4696,7 @@
         <v>30.89274</v>
       </c>
       <c r="J106" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K106" t="s">
         <v>8</v>
@@ -4746,7 +4746,7 @@
         <v>27.167629999999999</v>
       </c>
       <c r="J107" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K107" t="s">
         <v>8</v>
@@ -4796,7 +4796,7 @@
         <v>24.85549</v>
       </c>
       <c r="J108" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K108" t="s">
         <v>8</v>
@@ -4846,7 +4846,7 @@
         <v>20.680800000000001</v>
       </c>
       <c r="J109" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K109" t="s">
         <v>8</v>
@@ -4896,7 +4896,7 @@
         <v>14.32241</v>
       </c>
       <c r="J110" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K110" t="s">
         <v>8</v>
@@ -4946,7 +4946,7 @@
         <v>10.918430000000001</v>
       </c>
       <c r="J111" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K111" t="s">
         <v>8</v>
@@ -4996,7 +4996,7 @@
         <v>9.6981400000000004</v>
       </c>
       <c r="J112" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K112" t="s">
         <v>8</v>
@@ -5046,7 +5046,7 @@
         <v>8.4778400000000005</v>
       </c>
       <c r="J113" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K113" t="s">
         <v>8</v>
@@ -5096,7 +5096,7 @@
         <v>12.0745</v>
       </c>
       <c r="J114" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K114" t="s">
         <v>8</v>
@@ -5146,7 +5146,7 @@
         <v>33.396949999999997</v>
       </c>
       <c r="J115" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K115" t="s">
         <v>8</v>
@@ -5196,7 +5196,7 @@
         <v>32.951650000000001</v>
       </c>
       <c r="J116" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K116" t="s">
         <v>12</v>
@@ -5246,7 +5246,7 @@
         <v>31.99746</v>
       </c>
       <c r="J117" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K117" t="s">
         <v>12</v>
@@ -5296,7 +5296,7 @@
         <v>28.816790000000001</v>
       </c>
       <c r="J118" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K118" t="s">
         <v>12</v>
@@ -5346,7 +5346,7 @@
         <v>23.473279999999999</v>
       </c>
       <c r="J119" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K119" t="s">
         <v>12</v>
@@ -5396,7 +5396,7 @@
         <v>18.95674</v>
       </c>
       <c r="J120" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K120" t="s">
         <v>12</v>
@@ -5446,7 +5446,7 @@
         <v>15.585240000000001</v>
       </c>
       <c r="J121" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K121" t="s">
         <v>12</v>
@@ -5496,7 +5496,7 @@
         <v>12.78626</v>
       </c>
       <c r="J122" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K122" t="s">
         <v>12</v>
@@ -5546,7 +5546,7 @@
         <v>8.58779</v>
       </c>
       <c r="J123" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K123" t="s">
         <v>12</v>
@@ -5596,7 +5596,7 @@
         <v>11.195930000000001</v>
       </c>
       <c r="J124" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K124" t="s">
         <v>12</v>
@@ -5646,7 +5646,7 @@
         <v>25.12171</v>
       </c>
       <c r="J125" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K125" t="s">
         <v>12</v>
@@ -5696,10 +5696,10 @@
         <v>24.537489999999998</v>
       </c>
       <c r="J126" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K126" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L126">
         <v>5000</v>
@@ -5746,10 +5746,10 @@
         <v>22.687439999999999</v>
       </c>
       <c r="J127" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K127" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L127">
         <v>5000</v>
@@ -5796,10 +5796,10 @@
         <v>22.395330000000001</v>
       </c>
       <c r="J128" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K128" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L128">
         <v>5000</v>
@@ -5846,10 +5846,10 @@
         <v>18.695229999999999</v>
       </c>
       <c r="J129" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K129" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L129">
         <v>5000</v>
@@ -5896,10 +5896,10 @@
         <v>15.092499999999999</v>
       </c>
       <c r="J130" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K130" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L130">
         <v>5000</v>
@@ -5946,10 +5946,10 @@
         <v>12.755599999999999</v>
       </c>
       <c r="J131" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K131" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L131">
         <v>5000</v>
@@ -5996,10 +5996,10 @@
         <v>12.17137</v>
       </c>
       <c r="J132" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K132" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L132">
         <v>5000</v>
@@ -6046,10 +6046,10 @@
         <v>6.7186000000000003</v>
       </c>
       <c r="J133" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K133" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L133">
         <v>5000</v>
@@ -6096,10 +6096,10 @@
         <v>4.1869500000000004</v>
       </c>
       <c r="J134" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K134" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L134">
         <v>5000</v>
@@ -6146,10 +6146,10 @@
         <v>35.457920000000001</v>
       </c>
       <c r="J135" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K135" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L135">
         <v>5000</v>
@@ -6196,10 +6196,10 @@
         <v>34.405940000000001</v>
       </c>
       <c r="J136" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K136" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L136">
         <v>5000</v>
@@ -6246,10 +6246,10 @@
         <v>33.353960000000001</v>
       </c>
       <c r="J137" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K137" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L137">
         <v>5000</v>
@@ -6296,10 +6296,10 @@
         <v>31.745049999999999</v>
       </c>
       <c r="J138" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K138" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L138">
         <v>5000</v>
@@ -6346,10 +6346,10 @@
         <v>27.59901</v>
       </c>
       <c r="J139" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K139" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L139">
         <v>5000</v>
@@ -6396,10 +6396,10 @@
         <v>23.0198</v>
       </c>
       <c r="J140" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K140" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L140">
         <v>5000</v>
@@ -6446,10 +6446,10 @@
         <v>17.574259999999999</v>
       </c>
       <c r="J141" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K141" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L141">
         <v>5000</v>
@@ -6496,10 +6496,10 @@
         <v>12.06683</v>
       </c>
       <c r="J142" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K142" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L142">
         <v>5000</v>
@@ -6546,10 +6546,10 @@
         <v>12.623760000000001</v>
       </c>
       <c r="J143" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K143" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L143">
         <v>5000</v>
@@ -6596,10 +6596,10 @@
         <v>11.324260000000001</v>
       </c>
       <c r="J144" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K144" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L144">
         <v>5000</v>
@@ -6646,10 +6646,10 @@
         <v>50.662979999999997</v>
       </c>
       <c r="J145" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K145" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L145">
         <v>5000</v>
@@ -6696,10 +6696,10 @@
         <v>47.403309999999998</v>
       </c>
       <c r="J146" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K146" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L146">
         <v>10000</v>
@@ -6746,10 +6746,10 @@
         <v>45.027619999999999</v>
       </c>
       <c r="J147" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K147" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L147">
         <v>10000</v>
@@ -6796,10 +6796,10 @@
         <v>42.209940000000003</v>
       </c>
       <c r="J148" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K148" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L148">
         <v>10000</v>
@@ -6846,10 +6846,10 @@
         <v>39.558010000000003</v>
       </c>
       <c r="J149" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K149" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L149">
         <v>10000</v>
@@ -6896,10 +6896,10 @@
         <v>37.127070000000003</v>
       </c>
       <c r="J150" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K150" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L150">
         <v>10000</v>
@@ -6946,10 +6946,10 @@
         <v>33.922649999999997</v>
       </c>
       <c r="J151" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K151" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L151">
         <v>10000</v>
@@ -6996,10 +6996,10 @@
         <v>26.187850000000001</v>
       </c>
       <c r="J152" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K152" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L152">
         <v>10000</v>
@@ -7046,10 +7046,10 @@
         <v>21.43646</v>
       </c>
       <c r="J153" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K153" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L153">
         <v>10000</v>
@@ -7096,10 +7096,10 @@
         <v>19.39227</v>
       </c>
       <c r="J154" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K154" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L154">
         <v>10000</v>
@@ -7146,10 +7146,10 @@
         <v>48.5351</v>
       </c>
       <c r="J155" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K155" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L155">
         <v>10000</v>
@@ -7196,10 +7196,10 @@
         <v>45.771140000000003</v>
       </c>
       <c r="J156" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K156" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L156">
         <v>10000</v>
@@ -7246,10 +7246,10 @@
         <v>42.786070000000002</v>
       </c>
       <c r="J157" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K157" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L157">
         <v>10000</v>
@@ -7296,10 +7296,10 @@
         <v>41.127690000000001</v>
       </c>
       <c r="J158" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K158" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L158">
         <v>10000</v>
@@ -7346,10 +7346,10 @@
         <v>39.248199999999997</v>
       </c>
       <c r="J159" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K159" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L159">
         <v>10000</v>
@@ -7396,10 +7396,10 @@
         <v>36.097290000000001</v>
       </c>
       <c r="J160" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K160" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L160">
         <v>10000</v>
@@ -7446,10 +7446,10 @@
         <v>32.669980000000002</v>
       </c>
       <c r="J161" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K161" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L161">
         <v>10000</v>
@@ -7496,10 +7496,10 @@
         <v>23.10669</v>
       </c>
       <c r="J162" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K162" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L162">
         <v>10000</v>
@@ -7546,10 +7546,10 @@
         <v>22.498619999999999</v>
       </c>
       <c r="J163" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K163" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L163">
         <v>10000</v>
@@ -7596,10 +7596,10 @@
         <v>19.568819999999999</v>
       </c>
       <c r="J164" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K164" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L164">
         <v>10000</v>
@@ -7622,10 +7622,10 @@
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="J165" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K165" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L165">
         <v>10000</v>
@@ -7659,10 +7659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7685,7 +7685,7 @@
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
       <c r="K1" s="16" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="L1" s="16"/>
       <c r="M1" s="16"/>
@@ -8411,6 +8411,78 @@
       </c>
       <c r="E30" t="s">
         <v>17</v>
+      </c>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31" s="3">
+        <v>443</v>
+      </c>
+      <c r="M31" s="3">
+        <v>-1</v>
+      </c>
+      <c r="N31" s="6">
+        <v>9.6981400000000004</v>
+      </c>
+      <c r="O31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L32" s="3">
+        <v>428</v>
+      </c>
+      <c r="M32" s="3">
+        <v>-1</v>
+      </c>
+      <c r="N32" s="6">
+        <v>56.106870000000001</v>
+      </c>
+      <c r="O32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="11:15" x14ac:dyDescent="0.3">
+      <c r="K33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L33" s="4">
+        <v>190</v>
+      </c>
+      <c r="M33" s="4">
+        <v>-1</v>
+      </c>
+      <c r="N33" s="7">
+        <v>17.513809999999999</v>
+      </c>
+      <c r="O33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="11:15" x14ac:dyDescent="0.3">
+      <c r="K34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L34" s="4">
+        <v>191</v>
+      </c>
+      <c r="M34" s="4">
+        <v>-1</v>
+      </c>
+      <c r="N34" s="7">
+        <v>90.049750000000003</v>
+      </c>
+      <c r="O34" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -8427,7 +8499,7 @@
   <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8440,7 +8512,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -8462,7 +8534,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="5">
         <v>50</v>
@@ -8476,7 +8548,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5">
         <v>50</v>
@@ -8490,7 +8562,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5">
         <v>50</v>
@@ -8504,7 +8576,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5">
         <v>50</v>
@@ -8518,7 +8590,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="5">
         <v>50</v>
@@ -8532,7 +8604,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="5">
         <v>50</v>
@@ -8546,7 +8618,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="5">
         <v>50</v>
@@ -8560,7 +8632,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5">
         <v>50</v>
@@ -8574,7 +8646,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="5">
         <v>50</v>
@@ -8588,7 +8660,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="5">
         <v>50</v>
@@ -8608,7 +8680,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="5">
         <v>100</v>
@@ -8622,7 +8694,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5">
         <v>100</v>
@@ -8636,7 +8708,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="5">
         <v>100</v>
@@ -8650,7 +8722,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="5">
         <v>100</v>
@@ -8664,7 +8736,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="5">
         <v>100</v>
@@ -8678,7 +8750,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5">
         <v>100</v>
@@ -8692,7 +8764,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="5">
         <v>100</v>
@@ -8706,7 +8778,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="5">
         <v>100</v>
@@ -8720,7 +8792,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="5">
         <v>100</v>
@@ -8734,7 +8806,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="5">
         <v>100</v>
@@ -8754,7 +8826,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="5">
         <v>200</v>
@@ -8768,7 +8840,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="5">
         <v>200</v>
@@ -8782,7 +8854,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="5">
         <v>200</v>
@@ -8796,7 +8868,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="5">
         <v>200</v>
@@ -8810,7 +8882,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="5">
         <v>200</v>
@@ -8824,7 +8896,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="5">
         <v>200</v>
@@ -8838,7 +8910,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="5">
         <v>200</v>
@@ -8852,7 +8924,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="5">
         <v>200</v>
@@ -8866,7 +8938,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="5">
         <v>200</v>
@@ -8880,7 +8952,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="5">
         <v>200</v>
@@ -8900,7 +8972,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="5">
         <v>500</v>
@@ -8914,7 +8986,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="5">
         <v>500</v>
@@ -8928,7 +9000,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" s="5">
         <v>500</v>
@@ -8942,7 +9014,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="5">
         <v>500</v>
@@ -8956,7 +9028,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="5">
         <v>500</v>
@@ -8970,7 +9042,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B41" s="5">
         <v>500</v>
@@ -8984,7 +9056,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B42" s="5">
         <v>500</v>
@@ -8998,7 +9070,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B43" s="5">
         <v>500</v>
@@ -9012,7 +9084,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B44" s="5">
         <v>500</v>
@@ -9026,7 +9098,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B45" s="5">
         <v>500</v>
@@ -9046,7 +9118,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B47" s="5">
         <v>1000</v>
@@ -9060,7 +9132,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" s="5">
         <v>1000</v>
@@ -9074,7 +9146,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B49" s="5">
         <v>1000</v>
@@ -9088,7 +9160,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B50" s="5">
         <v>1000</v>
@@ -9102,7 +9174,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B51" s="5">
         <v>1000</v>
@@ -9116,7 +9188,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B52" s="5">
         <v>1000</v>
@@ -9130,7 +9202,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B53" s="5">
         <v>1000</v>
@@ -9144,7 +9216,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" s="5">
         <v>1000</v>
@@ -9158,7 +9230,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B55" s="5">
         <v>1000</v>
@@ -9172,7 +9244,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B56" s="5">
         <v>1000</v>
@@ -9192,7 +9264,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B58" s="5">
         <v>1400</v>
@@ -9206,7 +9278,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B59" s="5">
         <v>1400</v>
@@ -9220,7 +9292,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B60" s="5">
         <v>1400</v>
@@ -9234,7 +9306,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B61" s="5">
         <v>1400</v>
@@ -9248,7 +9320,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B62" s="5">
         <v>1400</v>
@@ -9262,7 +9334,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B63" s="5">
         <v>1400</v>
@@ -9276,7 +9348,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B64" s="5">
         <v>1400</v>
@@ -9290,7 +9362,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B65" s="5">
         <v>1400</v>
@@ -9304,7 +9376,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B66" s="5">
         <v>1400</v>
@@ -9318,7 +9390,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B67" s="5">
         <v>1400</v>

</xml_diff>